<commit_message>
added events and follow up events. as well as updated stats bars
</commit_message>
<xml_diff>
--- a/assets/events.xlsx
+++ b/assets/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\OneDrive\Desktop\YEAR 5\GameDesign\LyfeCraft\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{687F93D0-F3B4-44A1-8F8E-946025D78CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA25AB0B-13B1-40DA-93AC-0240A72E7BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="9084" xr2:uid="{8B60F0D8-E689-4C01-B640-F8CCAF006151}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B60F0D8-E689-4C01-B640-F8CCAF006151}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Event</t>
   </si>
@@ -62,64 +62,160 @@
     <t>Adventure</t>
   </si>
   <si>
-    <t>You walked across the street and found a lottery ticket on the floor! Do you pick it up or do you leave it be?</t>
-  </si>
-  <si>
     <t>Congrats! The lottery ticket was the winning ticket and you won $50000!</t>
   </si>
   <si>
-    <t>While hiking, you stumble upon a hidden cave. Do you explore it or continue on your path?</t>
-  </si>
-  <si>
-    <t>You find ancient treasures inside the cave worth $10,000!</t>
-  </si>
-  <si>
-    <t>You encounter a stray dog on the street. Do you ignore it or try to help it?</t>
-  </si>
-  <si>
-    <t>You successfully rescue the dog and find a grateful owner who rewards you with $100.</t>
-  </si>
-  <si>
-    <t>Your friend invites you to a high-stakes poker game. Do you join them or decline?</t>
-  </si>
-  <si>
-    <t>You win the poker game and walk away with $2000 in winnings!</t>
-  </si>
-  <si>
-    <t>While on a road trip, your car breaks down in the middle of nowhere. Do you try to fix it yourself or call for roadside assistance?</t>
-  </si>
-  <si>
-    <t>You manage to fix the car, saving yourself $200 in towing fees.</t>
-  </si>
-  <si>
-    <t>You receive an unexpected inheritance from a distant relative. Do you use it wisely or splurge on luxury items?</t>
-  </si>
-  <si>
-    <t>You invest the inheritance wisely and double your money in a year!</t>
-  </si>
-  <si>
-    <t>You get into an argument with your significant other. Do you apologize or let the tension linger?</t>
-  </si>
-  <si>
-    <t>You apologize and make up, strengthening your relationship.</t>
-  </si>
-  <si>
-    <t>A sudden illness lands you in the hospital. Do you have good insurance or will this be financially devastating?</t>
-  </si>
-  <si>
-    <t>Fortunately, you have good insurance coverage, and the medical bills are fully covered.</t>
-  </si>
-  <si>
-    <t>You decide to pursue further education. Do you take out a loan or find alternative means to fund your studies?</t>
-  </si>
-  <si>
-    <t>You receive a scholarship that covers your tuition fees completely!</t>
-  </si>
-  <si>
-    <t>A friend invites you on a spontaneous trip overseas. Do you take the opportunity or play it safe?</t>
-  </si>
-  <si>
-    <t>You have an unforgettable adventure and gain valuable life experiences.</t>
+    <t>You find a lottery ticket on the floor. Do you pick it up?</t>
+  </si>
+  <si>
+    <t>You come across an old, abandoned cabin in a dark forest. Do you enter?</t>
+  </si>
+  <si>
+    <t>Inside the cabin, you discover a hidden chest filled with ancient artifacts! Your adventurous spirit pays off as you gain valuable treasures.</t>
+  </si>
+  <si>
+    <t>A sudden storm hits while camping in the wilderness. Do you seek shelter?</t>
+  </si>
+  <si>
+    <t>Seeking shelter, you find a cave and encounter a lost traveler who offers you valuable survival skills. Your resourcefulness helps you weather the storm.</t>
+  </si>
+  <si>
+    <t>You stumble upon a hidden dungeon in an ancient castle. Do you explore it?</t>
+  </si>
+  <si>
+    <t>Exploring the dungeon, you encounter a cursed artifact that drains your vitality. However, you manage to escape, albeit weakened.</t>
+  </si>
+  <si>
+    <t>While traveling through a bustling marketplace, you witness a thief stealing from a merchant. Do you intervene?</t>
+  </si>
+  <si>
+    <t>You intervene and successfully apprehend the thief, earning the gratitude of the merchant. However, in the scuffle, you sustain minor injuries.</t>
+  </si>
+  <si>
+    <t>You attempt to capture the bird, but it eludes you, leading you on an exhilarating chase through the wilderness. While you don't catch the bird, you gain valuable insights into its behavior.</t>
+  </si>
+  <si>
+    <t>During a mountain hike, you encounter a rare species of bird. Do you attempt to catch it?</t>
+  </si>
+  <si>
+    <t>You receive an anonymous letter inviting you to a mysterious masquerade ball. Do you accept the invitation?</t>
+  </si>
+  <si>
+    <t>At the ball, you meet a wealthy benefactor who offers you a lucrative business opportunity.</t>
+  </si>
+  <si>
+    <t>While exploring a cave, you encounter a hidden treasure chest. Do you open it?</t>
+  </si>
+  <si>
+    <t>Inside the chest, you find valuable gems and artifacts worth a small fortune.</t>
+  </si>
+  <si>
+    <t>You overhear a conversation about a secret underground fighting ring. Do you investigate further?</t>
+  </si>
+  <si>
+    <t>You discover the fighting ring and participate in a high-stakes match, winning a substantial cash prize.</t>
+  </si>
+  <si>
+    <t>During a camping trip, you encounter a wounded wild animal. Do you try to help it?</t>
+  </si>
+  <si>
+    <t>You successfully nurse the animal back to health, earning the respect of local wildlife enthusiasts.</t>
+  </si>
+  <si>
+    <t>While exploring a haunted mansion, you encounter a ghostly apparition. Do you try to communicate with it?</t>
+  </si>
+  <si>
+    <t>The ghost reveals a hidden treasure buried on the mansion grounds, leading to a lucrative discovery.</t>
+  </si>
+  <si>
+    <t>You stumble upon an ancient map rumored to lead to buried treasure. Do you follow the map's directions?</t>
+  </si>
+  <si>
+    <t>Following the map, you discover a hidden cache of gold coins and precious jewels.</t>
+  </si>
+  <si>
+    <t>While hiking in the mountains, you encounter a group of stranded climbers. Do you offer assistance?</t>
+  </si>
+  <si>
+    <t>You help the climbers reach safety, forging strong bonds of friendship and gratitude.</t>
+  </si>
+  <si>
+    <t>During a deep-sea diving expedition, you discover a sunken shipwreck. Do you explore it?</t>
+  </si>
+  <si>
+    <t>Inside the shipwreck, you find valuable artifacts and treasures lost to the depths.</t>
+  </si>
+  <si>
+    <t>You witness an altercation between two rival gangs in the city streets. Do you intervene to break it up?</t>
+  </si>
+  <si>
+    <t>Your intervention prevents a violent clash, earning you respect and admiration from the community.</t>
+  </si>
+  <si>
+    <t>While volunteering at a local charity event, you meet a wealthy philanthropist. Do you strike up a conversation?</t>
+  </si>
+  <si>
+    <t>The philanthropist is impressed by your dedication and offers to fund your education or business venture.</t>
+  </si>
+  <si>
+    <t>You receive a suspicious email offering easy money if you provide your personal information. Do you respond to it?</t>
+  </si>
+  <si>
+    <t>Falling victim to a phishing scam, you lose a significant amount of money from your bank account.</t>
+  </si>
+  <si>
+    <t>While exploring a dark alley, you encounter a group of thugs. Do you confront them?</t>
+  </si>
+  <si>
+    <t>The thugs overpower you, leaving you injured and robbed of your possessions.</t>
+  </si>
+  <si>
+    <t>You're offered a shortcut to success through an unethical business proposition. Do you accept it?</t>
+  </si>
+  <si>
+    <t>Getting involved in the shady business deal, you face legal repercussions and damage to your reputation.</t>
+  </si>
+  <si>
+    <t>During a solo hiking trip, you become lost in the wilderness. Do you panic and wander aimlessly?</t>
+  </si>
+  <si>
+    <t>Lost and disoriented, you suffer from dehydration and exhaustion before being rescued.</t>
+  </si>
+  <si>
+    <t>While exploring an abandoned building, you trigger a collapse. Do you attempt to escape or freeze in fear?</t>
+  </si>
+  <si>
+    <t>Trapped beneath the rubble, you sustain severe injuries and require lengthy medical treatment.</t>
+  </si>
+  <si>
+    <t>You get involved in a toxic relationship despite warning signs. Do you stay in it hoping for change?</t>
+  </si>
+  <si>
+    <t>The relationship deteriorates further, leading to emotional trauma and a loss of self-worth.</t>
+  </si>
+  <si>
+    <t>You're persuaded to join a dangerous expedition without proper preparation. Do you go along with it?</t>
+  </si>
+  <si>
+    <t>The expedition ends in disaster, resulting in injuries, financial loss, and damaged equipment.</t>
+  </si>
+  <si>
+    <t>You ignore warnings and swim in a restricted area known for dangerous currents. Do you proceed?</t>
+  </si>
+  <si>
+    <t>Caught in a powerful undertow, you narrowly escape drowning but suffer injuries and trauma.</t>
+  </si>
+  <si>
+    <t>You lend a significant amount of money to a friend without a written agreement. Do you expect repayment?</t>
+  </si>
+  <si>
+    <t>Your friend fails to repay the loan, straining your relationship and causing financial hardship.</t>
+  </si>
+  <si>
+    <t>You ignore health warnings and indulge in excessive risky behavior. Do you continue down this path?</t>
+  </si>
+  <si>
+    <t>Your reckless behavior leads to serious health issues and long-term consequences.</t>
   </si>
 </sst>
 </file>
@@ -136,29 +232,24 @@
     </font>
     <font>
       <sz val="9.6"/>
-      <color rgb="FFECECEC"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9.6"/>
-      <color rgb="FFECECEC"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF212121"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -225,18 +316,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -573,13 +665,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1CC961-CEF9-4858-95C8-A47192ADBF2A}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="13.6640625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -607,287 +706,689 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="180" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
+        <v>50</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>-10</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-10</v>
+      </c>
+      <c r="H2" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>70</v>
+      </c>
+      <c r="D3" s="4">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-20</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-10</v>
+      </c>
+      <c r="H4" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>-50</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-20</v>
+      </c>
+      <c r="H5" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>50</v>
+      </c>
+      <c r="G7" s="4">
+        <v>20</v>
+      </c>
+      <c r="H7" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4">
+        <v>80</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>50</v>
+      </c>
+      <c r="F8" s="4">
+        <v>-20</v>
+      </c>
+      <c r="G8" s="4">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>-10</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>-20</v>
+      </c>
+      <c r="G10" s="4">
+        <v>20</v>
+      </c>
+      <c r="H10" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4">
+        <v>40</v>
+      </c>
+      <c r="F11" s="4">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4">
+        <v>70</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>-10</v>
+      </c>
+      <c r="G12" s="4">
+        <v>20</v>
+      </c>
+      <c r="H12" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4">
         <v>90</v>
       </c>
-      <c r="D2" s="3">
-        <v>-2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>-2</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-30</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4">
+        <v>60</v>
+      </c>
+      <c r="F14" s="4">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="4">
+        <v>80</v>
+      </c>
+      <c r="D15" s="4">
+        <v>20</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-20</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4">
+        <v>50</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>20</v>
+      </c>
+      <c r="H16" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>70</v>
+      </c>
+      <c r="F17" s="4">
+        <v>40</v>
+      </c>
+      <c r="G17" s="4">
+        <v>30</v>
+      </c>
+      <c r="H17" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4">
+        <v>-80</v>
+      </c>
+      <c r="D18" s="4">
         <v>-10</v>
       </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="180" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>80</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-5</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
-        <v>60</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3">
-        <v>-5</v>
-      </c>
-      <c r="G4" s="3">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3">
-        <v>85</v>
-      </c>
-      <c r="D5" s="3">
-        <v>-5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E18" s="4">
+        <v>-50</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-30</v>
+      </c>
+      <c r="G18" s="4">
+        <v>-50</v>
+      </c>
+      <c r="H18" s="5">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4">
+        <v>-70</v>
+      </c>
+      <c r="D19" s="4">
+        <v>-30</v>
+      </c>
+      <c r="E19" s="4">
+        <v>-40</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>-40</v>
+      </c>
+      <c r="H19" s="5">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="4">
+        <v>-90</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>-60</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-20</v>
+      </c>
+      <c r="G20" s="4">
+        <v>-80</v>
+      </c>
+      <c r="H20" s="5">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>-60</v>
+      </c>
+      <c r="E21" s="4">
+        <v>-30</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>-20</v>
+      </c>
+      <c r="H21" s="5">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="4">
+        <v>-60</v>
+      </c>
+      <c r="D22" s="4">
+        <v>-80</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
         <v>-10</v>
       </c>
-      <c r="G5" s="3">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3">
-        <v>70</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-10</v>
-      </c>
-      <c r="E6" s="3">
-        <v>-5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3">
-        <v>100</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3">
-        <v>10</v>
-      </c>
-      <c r="H7" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3">
-        <v>75</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3">
-        <v>80</v>
-      </c>
-      <c r="D9" s="3">
-        <v>-15</v>
-      </c>
-      <c r="E9" s="3">
-        <v>-5</v>
-      </c>
-      <c r="F9" s="3">
-        <v>-10</v>
-      </c>
-      <c r="G9" s="3">
-        <v>-5</v>
-      </c>
-      <c r="H9" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3">
-        <v>60</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>15</v>
-      </c>
-      <c r="G10" s="3">
-        <v>5</v>
-      </c>
-      <c r="H10" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3">
-        <v>70</v>
-      </c>
-      <c r="D11" s="3">
-        <v>-5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3">
-        <v>-5</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <v>30</v>
+      <c r="G22" s="4">
+        <v>-30</v>
+      </c>
+      <c r="H22" s="5">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>-40</v>
+      </c>
+      <c r="E23" s="4">
+        <v>-90</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="4">
+        <v>-70</v>
+      </c>
+      <c r="D24" s="4">
+        <v>-50</v>
+      </c>
+      <c r="E24" s="4">
+        <v>-20</v>
+      </c>
+      <c r="F24" s="4">
+        <v>-30</v>
+      </c>
+      <c r="G24" s="4">
+        <v>-40</v>
+      </c>
+      <c r="H24" s="5">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>-80</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>-20</v>
+      </c>
+      <c r="H25" s="5">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="4">
+        <v>-90</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>-70</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>-100</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>-80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F8BEB6B91115244B0F57877C9E4273C" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426ba5ee42f294db52d085105e1378ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2ca2bca3-7074-49c7-81e0-dd5bcc1fa2e3" xmlns:ns4="57a0d5aa-09bb-4712-a2c3-205855705b70" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec59f48a7948fd0740026127c66ff042" ns3:_="" ns4:_="">
     <xsd:import namespace="2ca2bca3-7074-49c7-81e0-dd5bcc1fa2e3"/>
@@ -1058,32 +1559,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{912DB088-39AB-4F6E-A4CB-285820F15040}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="57a0d5aa-09bb-4712-a2c3-205855705b70"/>
-    <ds:schemaRef ds:uri="2ca2bca3-7074-49c7-81e0-dd5bcc1fa2e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C2B4F2-F63B-4089-8A79-CA34B56B333A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD519816-B5EC-4F8C-B24C-C7E15B312F35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1100,4 +1591,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C2B4F2-F63B-4089-8A79-CA34B56B333A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{912DB088-39AB-4F6E-A4CB-285820F15040}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="57a0d5aa-09bb-4712-a2c3-205855705b70"/>
+    <ds:schemaRef ds:uri="2ca2bca3-7074-49c7-81e0-dd5bcc1fa2e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>